<commit_message>
New test being made
</commit_message>
<xml_diff>
--- a/tickers2.xlsx
+++ b/tickers2.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dissertation Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dissertation Project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99F989D-3B2D-4161-929A-6B59253C0C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F0B36B-6C47-483E-B8A4-D6467A90A18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="204">
   <si>
     <t>Rank</t>
   </si>
@@ -1010,16 +1011,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1089,7 +1092,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>124</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>140</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -1551,7 +1554,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>156</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>160</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>164</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>168</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>172</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>176</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>180</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>184</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>188</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>192</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>196</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>200</v>
       </c>
@@ -1739,4 +1742,103 @@
     <ignoredError sqref="A1:E53" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088713AA-04FB-46CD-B3FB-7585A24702F6}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed getting dates, need to fix calcs
</commit_message>
<xml_diff>
--- a/tickers2.xlsx
+++ b/tickers2.xlsx
@@ -5,23 +5,24 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Dissertation Project\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Taahaa\projects\StockSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0036A57B-DAD2-4B2D-B954-FD021E7F7141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E31A4E-184B-45B8-9B5E-02CCB337EDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="204">
   <si>
     <t>Rank</t>
   </si>
@@ -1748,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088713AA-04FB-46CD-B3FB-7585A24702F6}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1841,4 +1842,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB70493-9931-4107-8796-0D332C383901}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Timing and selection fixed, db implementation now
</commit_message>
<xml_diff>
--- a/tickers2.xlsx
+++ b/tickers2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proje\Desktop\projects\StockSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Taahaa\projects\StockSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7852DD2-005C-491C-BAED-BCE37DC5BA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAD697F-B98D-408C-8DE6-534A39525A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>Meta Platforms, Inc.</t>
-  </si>
-  <si>
     <t>FB</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>UNITEDHEALTH GROUP INCORPORATED</t>
-  </si>
-  <si>
     <t>UNH</t>
   </si>
   <si>
@@ -231,9 +225,6 @@
     <t>17</t>
   </si>
   <si>
-    <t>MASTERCARD INCORPORATED.</t>
-  </si>
-  <si>
     <t>MA</t>
   </si>
   <si>
@@ -315,9 +306,6 @@
     <t>24</t>
   </si>
   <si>
-    <t>Broadcom Inc.</t>
-  </si>
-  <si>
     <t>AVGO</t>
   </si>
   <si>
@@ -399,9 +387,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>ACCENTURE PUBLIC LIMITED COMPANY</t>
-  </si>
-  <si>
     <t>ACN</t>
   </si>
   <si>
@@ -567,9 +552,6 @@
     <t>45</t>
   </si>
   <si>
-    <t>QUALCOMM INCORPORATED</t>
-  </si>
-  <si>
     <t>QCOM</t>
   </si>
   <si>
@@ -603,9 +585,6 @@
     <t>48</t>
   </si>
   <si>
-    <t>TEXAS INSTRUMENTS INCORPORATED</t>
-  </si>
-  <si>
     <t>TXN</t>
   </si>
   <si>
@@ -637,6 +616,27 @@
   </si>
   <si>
     <t>CompanyName</t>
+  </si>
+  <si>
+    <t>UNITEDHEALTH GROUP INC.</t>
+  </si>
+  <si>
+    <t>META PLATFORMS, INC.</t>
+  </si>
+  <si>
+    <t>BROADCOM INC.</t>
+  </si>
+  <si>
+    <t>QUALCOMM INC.</t>
+  </si>
+  <si>
+    <t>TEXAS INSTRUMENTS INC.</t>
+  </si>
+  <si>
+    <t>MASTERCARD INC.</t>
+  </si>
+  <si>
+    <t>ACCENTURE PLC.</t>
   </si>
 </sst>
 </file>
@@ -1015,23 +1015,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1040,7 +1040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1138,612 +1138,612 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
       <c r="B9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="B15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>65</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>66</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>69</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B19" t="s">
         <v>70</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C19" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="D19" t="s">
         <v>72</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>73</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
         <v>74</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="D20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>77</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B21" t="s">
         <v>78</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C21" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="D21" t="s">
         <v>80</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B22" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C22" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="D22" t="s">
         <v>84</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>85</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B23" t="s">
         <v>86</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="D23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>89</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B24" t="s">
         <v>90</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C24" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="D24" t="s">
         <v>92</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>93</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C25" t="s">
         <v>94</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>96</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>97</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>100</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>101</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>102</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>104</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>105</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>106</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>108</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>109</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>110</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>112</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>113</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>114</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>116</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>118</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>120</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" t="s">
         <v>121</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
         <v>122</v>
       </c>
-      <c r="D31" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
         <v>124</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C33" t="s">
         <v>125</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D33" t="s">
         <v>126</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="B34" t="s">
         <v>128</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C34" t="s">
         <v>129</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D34" t="s">
         <v>130</v>
       </c>
-      <c r="D33" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
         <v>132</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C35" t="s">
         <v>133</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D35" t="s">
         <v>134</v>
       </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="B36" t="s">
         <v>136</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C36" t="s">
         <v>137</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D36" t="s">
         <v>138</v>
       </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
         <v>140</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C37" t="s">
         <v>141</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D37" t="s">
         <v>142</v>
       </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="B38" t="s">
         <v>144</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C38" t="s">
         <v>145</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D38" t="s">
         <v>146</v>
       </c>
-      <c r="D37" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="B39" t="s">
         <v>148</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C39" t="s">
         <v>149</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D39" t="s">
         <v>150</v>
       </c>
-      <c r="D38" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="B40" t="s">
         <v>152</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C40" t="s">
         <v>153</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D40" t="s">
         <v>154</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
         <v>156</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C41" t="s">
         <v>157</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D41" t="s">
         <v>158</v>
       </c>
-      <c r="D40" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="B42" t="s">
         <v>160</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C42" t="s">
         <v>161</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D42" t="s">
         <v>162</v>
       </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="B43" t="s">
         <v>164</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C43" t="s">
         <v>165</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D43" t="s">
         <v>166</v>
       </c>
-      <c r="D42" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="B44" t="s">
         <v>168</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C44" t="s">
         <v>169</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D44" t="s">
         <v>170</v>
       </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="B45" t="s">
         <v>172</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C45" t="s">
         <v>173</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D45" t="s">
         <v>174</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="B46" t="s">
+        <v>201</v>
+      </c>
+      <c r="C46" t="s">
         <v>176</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D46" t="s">
         <v>177</v>
       </c>
-      <c r="C45" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>178</v>
       </c>
-      <c r="D45" t="s">
+      <c r="B47" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="C47" t="s">
         <v>180</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D47" t="s">
         <v>181</v>
       </c>
-      <c r="C46" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>182</v>
       </c>
-      <c r="D46" t="s">
+      <c r="B48" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="C48" t="s">
         <v>184</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D48" t="s">
         <v>185</v>
       </c>
-      <c r="C47" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>186</v>
       </c>
-      <c r="D47" t="s">
+      <c r="B49" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="D49" t="s">
         <v>188</v>
       </c>
-      <c r="B48" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>189</v>
       </c>
-      <c r="C48" t="s">
+      <c r="B50" t="s">
         <v>190</v>
       </c>
-      <c r="D48" t="s">
+      <c r="C50" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="D50" t="s">
         <v>192</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>193</v>
       </c>
-      <c r="C49" t="s">
+      <c r="B51" t="s">
         <v>194</v>
       </c>
-      <c r="D49" t="s">
+      <c r="C51" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="D51" t="s">
         <v>196</v>
-      </c>
-      <c r="B50" t="s">
-        <v>197</v>
-      </c>
-      <c r="C50" t="s">
-        <v>198</v>
-      </c>
-      <c r="D50" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>200</v>
-      </c>
-      <c r="B51" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51" t="s">
-        <v>202</v>
-      </c>
-      <c r="D51" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:E53 A1 C1:E1" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:E8 A1 C1:E1 A11:E17 A10 C10:E10 A9 C9:E9 A26:E31 A25 C25:E25 A50:E53 A49 C49:E49 A47:E48 A46 C46:E46 A19:E24 A18 C18:E18 A33:E45 A32 C32:E32" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1756,17 +1756,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1775,7 +1775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1854,16 +1854,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB70493-9931-4107-8796-0D332C383901}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Saving to db working
</commit_message>
<xml_diff>
--- a/tickers2.xlsx
+++ b/tickers2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Taahaa\projects\StockSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proje\Desktop\projects\StockSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAD697F-B98D-408C-8DE6-534A39525A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F865919-C806-4AB3-9319-0C5593E7AB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="210">
   <si>
     <t>Rank</t>
   </si>
@@ -99,9 +99,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>BERKSHIRE HATHAWAY INC.</t>
-  </si>
-  <si>
     <t>BRK.A</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>VISA INC.</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>13</t>
   </si>
   <si>
-    <t>WALMART INC.</t>
-  </si>
-  <si>
     <t>WMT</t>
   </si>
   <si>
@@ -189,9 +180,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>THE PROCTER &amp; GAMBLE COMPANY</t>
-  </si>
-  <si>
     <t>PG</t>
   </si>
   <si>
@@ -201,9 +189,6 @@
     <t>15</t>
   </si>
   <si>
-    <t>EXXON MOBIL CORPORATION</t>
-  </si>
-  <si>
     <t>XOM</t>
   </si>
   <si>
@@ -213,9 +198,6 @@
     <t>16</t>
   </si>
   <si>
-    <t>BANK OF AMERICA CORPORATION</t>
-  </si>
-  <si>
     <t>BAC</t>
   </si>
   <si>
@@ -234,9 +216,6 @@
     <t>18</t>
   </si>
   <si>
-    <t>CHEVRON CORPORATION</t>
-  </si>
-  <si>
     <t>CVX</t>
   </si>
   <si>
@@ -246,9 +225,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>THE HOME DEPOT, INC.</t>
-  </si>
-  <si>
     <t>HD</t>
   </si>
   <si>
@@ -258,9 +234,6 @@
     <t>20</t>
   </si>
   <si>
-    <t>PFIZER INC.</t>
-  </si>
-  <si>
     <t>PFE</t>
   </si>
   <si>
@@ -270,9 +243,6 @@
     <t>21</t>
   </si>
   <si>
-    <t>ABBVIE INC.</t>
-  </si>
-  <si>
     <t>ABBV</t>
   </si>
   <si>
@@ -294,9 +264,6 @@
     <t>23</t>
   </si>
   <si>
-    <t>THE COCA-COLA COMPANY</t>
-  </si>
-  <si>
     <t>KO</t>
   </si>
   <si>
@@ -315,9 +282,6 @@
     <t>25</t>
   </si>
   <si>
-    <t>THE WALT DISNEY COMPANY</t>
-  </si>
-  <si>
     <t>DIS</t>
   </si>
   <si>
@@ -327,9 +291,6 @@
     <t>26</t>
   </si>
   <si>
-    <t>COSTCO WHOLESALE CORPORATION</t>
-  </si>
-  <si>
     <t>COST</t>
   </si>
   <si>
@@ -339,9 +300,6 @@
     <t>27</t>
   </si>
   <si>
-    <t>PEPSICO, INC.</t>
-  </si>
-  <si>
     <t>PEP</t>
   </si>
   <si>
@@ -351,9 +309,6 @@
     <t>28</t>
   </si>
   <si>
-    <t>CISCO SYSTEMS, INC.</t>
-  </si>
-  <si>
     <t>CSCO</t>
   </si>
   <si>
@@ -363,9 +318,6 @@
     <t>29</t>
   </si>
   <si>
-    <t>THERMO FISHER SCIENTIFIC INC.</t>
-  </si>
-  <si>
     <t>TMO</t>
   </si>
   <si>
@@ -396,9 +348,6 @@
     <t>32</t>
   </si>
   <si>
-    <t>VERIZON COMMUNICATIONS INC.</t>
-  </si>
-  <si>
     <t>VZ</t>
   </si>
   <si>
@@ -408,9 +357,6 @@
     <t>33</t>
   </si>
   <si>
-    <t>COMCAST CORPORATION</t>
-  </si>
-  <si>
     <t>CMCSA</t>
   </si>
   <si>
@@ -420,9 +366,6 @@
     <t>34</t>
   </si>
   <si>
-    <t>NIKE, INC.</t>
-  </si>
-  <si>
     <t>NKE</t>
   </si>
   <si>
@@ -456,9 +399,6 @@
     <t>37</t>
   </si>
   <si>
-    <t>SALESFORCE.COM, INC.</t>
-  </si>
-  <si>
     <t>CRM</t>
   </si>
   <si>
@@ -480,9 +420,6 @@
     <t>39</t>
   </si>
   <si>
-    <t>MERCK &amp; CO., INC.</t>
-  </si>
-  <si>
     <t>MRK</t>
   </si>
   <si>
@@ -492,9 +429,6 @@
     <t>40</t>
   </si>
   <si>
-    <t>ADOBE INC.</t>
-  </si>
-  <si>
     <t>ADBE</t>
   </si>
   <si>
@@ -516,9 +450,6 @@
     <t>42</t>
   </si>
   <si>
-    <t>ADVANCED MICRO DEVICES, INC.</t>
-  </si>
-  <si>
     <t>AMD</t>
   </si>
   <si>
@@ -528,9 +459,6 @@
     <t>43</t>
   </si>
   <si>
-    <t>UNITED PARCEL SERVICE, INC.</t>
-  </si>
-  <si>
     <t>UPS</t>
   </si>
   <si>
@@ -540,9 +468,6 @@
     <t>44</t>
   </si>
   <si>
-    <t>MCDONALD'S CORPORATION</t>
-  </si>
-  <si>
     <t>MCD</t>
   </si>
   <si>
@@ -561,9 +486,6 @@
     <t>46</t>
   </si>
   <si>
-    <t>UNION PACIFIC CORPORATION</t>
-  </si>
-  <si>
     <t>UNP</t>
   </si>
   <si>
@@ -573,9 +495,6 @@
     <t>47</t>
   </si>
   <si>
-    <t>THE CHARLES SCHWAB CORPORATION</t>
-  </si>
-  <si>
     <t>SCHW</t>
   </si>
   <si>
@@ -594,9 +513,6 @@
     <t>49</t>
   </si>
   <si>
-    <t>AT&amp;T INC.</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -606,9 +522,6 @@
     <t>50</t>
   </si>
   <si>
-    <t>NETFLIX, INC.</t>
-  </si>
-  <si>
     <t>NFLX</t>
   </si>
   <si>
@@ -618,25 +531,127 @@
     <t>CompanyName</t>
   </si>
   <si>
-    <t>UNITEDHEALTH GROUP INC.</t>
-  </si>
-  <si>
-    <t>META PLATFORMS, INC.</t>
-  </si>
-  <si>
-    <t>BROADCOM INC.</t>
-  </si>
-  <si>
-    <t>QUALCOMM INC.</t>
-  </si>
-  <si>
-    <t>TEXAS INSTRUMENTS INC.</t>
-  </si>
-  <si>
-    <t>MASTERCARD INC.</t>
-  </si>
-  <si>
     <t>ACCENTURE PLC.</t>
+  </si>
+  <si>
+    <t>THE CHARLES SCHWAB CORP.</t>
+  </si>
+  <si>
+    <t>MICROSOFT</t>
+  </si>
+  <si>
+    <t>AMAZON.COM</t>
+  </si>
+  <si>
+    <t>TESLA</t>
+  </si>
+  <si>
+    <t>BERKSHIRE HATHAWAY</t>
+  </si>
+  <si>
+    <t>NETFLIX</t>
+  </si>
+  <si>
+    <t>AT&amp;T</t>
+  </si>
+  <si>
+    <t>TEXAS INSTRUMENTS</t>
+  </si>
+  <si>
+    <t>MCDONALD'S</t>
+  </si>
+  <si>
+    <t>ADVANCED MICRO DEVICES</t>
+  </si>
+  <si>
+    <t>ADOBE</t>
+  </si>
+  <si>
+    <t>MERCK &amp; CO</t>
+  </si>
+  <si>
+    <t>SALESFORCE.COM</t>
+  </si>
+  <si>
+    <t>NIKE</t>
+  </si>
+  <si>
+    <t>COMCAST</t>
+  </si>
+  <si>
+    <t>VERIZON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUALCOMM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALPHABET </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNITEDHEALTH GROUP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WALMART </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MASTERCARD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFIZER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABBVIE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BROADCOM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">THERMO FISHER SCIENTIFIC </t>
+  </si>
+  <si>
+    <t>META PLATFORMS</t>
+  </si>
+  <si>
+    <t>THE HOME DEPOT</t>
+  </si>
+  <si>
+    <t>UNITED PARCEL SERVICE</t>
+  </si>
+  <si>
+    <t>PROCTER &amp; GAMBLE</t>
+  </si>
+  <si>
+    <t>UNION PACIFIC</t>
+  </si>
+  <si>
+    <t>COSTCO WHOLESALE</t>
+  </si>
+  <si>
+    <t>COCA-COLA</t>
+  </si>
+  <si>
+    <t>WALT DISNEY</t>
+  </si>
+  <si>
+    <t>CISCO SYSTEMS</t>
+  </si>
+  <si>
+    <t>PEPSICO</t>
+  </si>
+  <si>
+    <t>BANK OF AMERICA</t>
+  </si>
+  <si>
+    <t>EXXON MOBIL</t>
+  </si>
+  <si>
+    <t>CHEVRON</t>
   </si>
 </sst>
 </file>
@@ -1015,23 +1030,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.58203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1040,12 +1055,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1054,12 +1069,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1068,12 +1083,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -1082,12 +1097,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -1096,12 +1111,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -1110,640 +1125,640 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
+        <v>185</v>
+      </c>
+      <c r="C33" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" t="s">
         <v>199</v>
       </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
-        <v>203</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" t="s">
-        <v>200</v>
-      </c>
-      <c r="C25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" t="s">
-        <v>204</v>
-      </c>
-      <c r="C32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B34" t="s">
-        <v>128</v>
-      </c>
-      <c r="C34" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>131</v>
-      </c>
-      <c r="B35" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" t="s">
-        <v>133</v>
-      </c>
-      <c r="D35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>135</v>
-      </c>
-      <c r="B36" t="s">
-        <v>136</v>
-      </c>
-      <c r="C36" t="s">
-        <v>137</v>
-      </c>
-      <c r="D36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>139</v>
-      </c>
-      <c r="B37" t="s">
-        <v>140</v>
-      </c>
-      <c r="C37" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>143</v>
-      </c>
-      <c r="B38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="C44" t="s">
         <v>145</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D44" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>147</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C45" t="s">
         <v>148</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D45" t="s">
         <v>149</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" t="s">
         <v>151</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D46" t="s">
         <v>152</v>
       </c>
-      <c r="C40" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>153</v>
       </c>
-      <c r="D40" t="s">
+      <c r="B47" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="D47" t="s">
         <v>155</v>
       </c>
-      <c r="B41" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>156</v>
       </c>
-      <c r="C41" t="s">
+      <c r="B48" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" t="s">
         <v>157</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D48" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>159</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B49" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" t="s">
         <v>160</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D49" t="s">
         <v>161</v>
       </c>
-      <c r="D42" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" t="s">
         <v>163</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D50" t="s">
         <v>164</v>
       </c>
-      <c r="C43" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>165</v>
       </c>
-      <c r="D43" t="s">
+      <c r="B51" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="D51" t="s">
         <v>167</v>
-      </c>
-      <c r="B44" t="s">
-        <v>168</v>
-      </c>
-      <c r="C44" t="s">
-        <v>169</v>
-      </c>
-      <c r="D44" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>171</v>
-      </c>
-      <c r="B45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C45" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>175</v>
-      </c>
-      <c r="B46" t="s">
-        <v>201</v>
-      </c>
-      <c r="C46" t="s">
-        <v>176</v>
-      </c>
-      <c r="D46" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>178</v>
-      </c>
-      <c r="B47" t="s">
-        <v>179</v>
-      </c>
-      <c r="C47" t="s">
-        <v>180</v>
-      </c>
-      <c r="D47" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>182</v>
-      </c>
-      <c r="B48" t="s">
-        <v>183</v>
-      </c>
-      <c r="C48" t="s">
-        <v>184</v>
-      </c>
-      <c r="D48" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>186</v>
-      </c>
-      <c r="B49" t="s">
-        <v>202</v>
-      </c>
-      <c r="C49" t="s">
-        <v>187</v>
-      </c>
-      <c r="D49" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>189</v>
-      </c>
-      <c r="B50" t="s">
-        <v>190</v>
-      </c>
-      <c r="C50" t="s">
-        <v>191</v>
-      </c>
-      <c r="D50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>193</v>
-      </c>
-      <c r="B51" t="s">
-        <v>194</v>
-      </c>
-      <c r="C51" t="s">
-        <v>195</v>
-      </c>
-      <c r="D51" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:E8 A1 C1:E1 A11:E17 A10 C10:E10 A9 C9:E9 A26:E31 A25 C25:E25 A50:E53 A49 C49:E49 A47:E48 A46 C46:E46 A19:E24 A18 C18:E18 A33:E45 A32 C32:E32" numberStoredAsText="1"/>
+    <ignoredError sqref="A2 A1 C1:E1 A11:E11 A10 C10:E10 A9 C9:E9 A26 A25 C25:E25 A50 A49 C49:E49 A47 A46 C46:E46 A19 A18 C18:E18 A33 A32 C32:E32 A48 C48:E48 A8:E8 A3 C3:E3 A4 C4:E4 A5 C5:E5 A6 C6:E6 A7 C7:E7 A52:E53 A51 C51:E51 C50:E50 A45 C45:E45 A44 A43 C43:E43 A42 A41 C41:E41 A40 C40:E40 C42:E42 A39:E39 A38 C38:E38 A36:E37 A34 C34:E34 A35 C35:E35 C33:E33 C44:E44 C2:E2 A13:E13 A12 C12:E12 A16 A14 C14:E14 A23:E23 A20 C20:E20 A21 C21:E21 A22 C22:E22 A31:E31 A28 C28:E28 A29 C29:E29 A30 C30:E30 A15 C15:E15 C47:E47 A27 C27:E27 A24 C24:E24 C26:E26 A17 C17:E17 C16:E16 C19:E19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1756,17 +1771,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1775,7 +1790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1789,7 +1804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1803,7 +1818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1817,7 +1832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1831,7 +1846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1858,12 +1873,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1877,7 +1892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>

</xml_diff>